<commit_message>
Titre fonctionnel et excel trié
</commit_message>
<xml_diff>
--- a/VideoBalles/ListeBalles.xlsx
+++ b/VideoBalles/ListeBalles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\tiktok_manager\VideoBalles\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\tiktok_manager\VideoBalles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7888DBBB-EDC1-4AB6-A782-F75FDCDC8107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE72E99-0D59-4F3D-9B9D-34D6DD132C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Couleur Balle</t>
   </si>
@@ -135,6 +135,66 @@
   </si>
   <si>
     <t>Couleur Texte Score</t>
+  </si>
+  <si>
+    <t>Pays - Bas</t>
+  </si>
+  <si>
+    <t>PaysBas.png</t>
+  </si>
+  <si>
+    <t>PSG</t>
+  </si>
+  <si>
+    <t>PSG.png</t>
+  </si>
+  <si>
+    <t>Chelsea_FC.png</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Sinner</t>
+  </si>
+  <si>
+    <t>SINNER</t>
+  </si>
+  <si>
+    <t>Sinner.jpg</t>
+  </si>
+  <si>
+    <t>Alcaraz.png</t>
+  </si>
+  <si>
+    <t>Alcaraz</t>
+  </si>
+  <si>
+    <t>(219,161,17)</t>
+  </si>
+  <si>
+    <t>CHE</t>
+  </si>
+  <si>
+    <t>NED</t>
+  </si>
+  <si>
+    <t>ALCARAZ</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>Oui / Non</t>
+  </si>
+  <si>
+    <t>Foot - Pays</t>
+  </si>
+  <si>
+    <t>Foot - Club</t>
+  </si>
+  <si>
+    <t>Tennis</t>
   </si>
 </sst>
 </file>
@@ -170,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -181,11 +241,34 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -220,13 +303,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -264,24 +340,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:O6">
-  <autoFilter ref="A1:O6" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:P13">
+  <autoFilter ref="A1:P13" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{CF5BAF0D-2A1A-45F2-8436-156371C73BFB}" name="Catégorie" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{08BE89D9-A157-4F06-A086-DFCD4C59CA11}" name="INFOS"/>
-    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{4350E952-AA26-4181-A722-64FC122F2526}" name="Couleur Balle"/>
-    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="7"/>
     <tableColumn id="13" xr3:uid="{FC727AA8-9DB1-4BCB-878B-78ACCB013E96}" name="Couleur Rectangle Score"/>
     <tableColumn id="14" xr3:uid="{631E6625-8583-4F25-B9D4-E2EE6798BD97}" name="Couleur Texte Score"/>
-    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon Balle" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon Balle" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{4F86DC08-4D23-48D4-B800-C3477A97072A}" name="Couleur Interieur Balle"/>
-    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainee" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainee" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,275 +681,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5B4434-761B-4D40-92E9-037B049A5ECC}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" style="3"/>
-    <col min="4" max="4" width="15.46484375" customWidth="1"/>
-    <col min="5" max="5" width="12.265625" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="23.265625" customWidth="1"/>
-    <col min="9" max="9" width="18.86328125" customWidth="1"/>
-    <col min="10" max="10" width="11.86328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="6.265625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.86328125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="2"/>
-    <col min="16" max="16" width="10.6640625" style="2"/>
-    <col min="18" max="18" width="22.33203125" customWidth="1"/>
-    <col min="19" max="19" width="20.06640625" customWidth="1"/>
-    <col min="20" max="20" width="12.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4"/>
+    <col min="4" max="4" width="10.6640625" style="3"/>
+    <col min="5" max="5" width="15.46484375" customWidth="1"/>
+    <col min="6" max="6" width="12.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" customWidth="1"/>
+    <col min="8" max="8" width="13.3984375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.265625" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" customWidth="1"/>
+    <col min="11" max="11" width="11.86328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.86328125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="2"/>
+    <col min="17" max="17" width="10.6640625" style="2"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="20" max="20" width="20.06640625" customWidth="1"/>
+    <col min="21" max="21" width="12.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1"/>
+      <c r="Q1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="b">
+      <c r="E2" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>2</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>10</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>25</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>0.3</v>
       </c>
-      <c r="P2"/>
+      <c r="Q2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>10</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>25</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>0.3</v>
       </c>
-      <c r="P3"/>
+      <c r="Q3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4"/>
+      <c r="E4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>10</v>
+      </c>
+      <c r="O5" s="2">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>10</v>
+      </c>
+      <c r="O6" s="2">
+        <v>25</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2">
+        <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>10</v>
+      </c>
+      <c r="O7" s="2">
+        <v>25</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="2">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L9" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M9" s="2">
         <v>2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N9" s="2">
         <v>10</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O9" s="2">
         <v>25</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P9" s="2">
         <v>0.3</v>
       </c>
-      <c r="P5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>10</v>
+      </c>
+      <c r="O10" s="2">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="P10" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
         <v>20</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L12" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M12" s="2">
         <v>2</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N12" s="2">
         <v>10</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O12" s="2">
         <v>25</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P12" s="2">
         <v>0.3</v>
       </c>
-      <c r="P6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2">
+        <v>20</v>
+      </c>
+      <c r="L13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>10</v>
+      </c>
+      <c r="O13" s="2">
+        <v>25</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fonctionnel avec titre qui informe sur le nom
</commit_message>
<xml_diff>
--- a/VideoBalles/ListeBalles.xlsx
+++ b/VideoBalles/ListeBalles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\tiktok_manager\VideoBalles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE72E99-0D59-4F3D-9B9D-34D6DD132C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B3666-8773-489A-8641-D35672DEF9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
+    <workbookView xWindow="5400" yWindow="2858" windowWidth="16200" windowHeight="9307" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>Couleur Balle</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>Tennis</t>
+  </si>
+  <si>
+    <t>(142,174,92)</t>
+  </si>
+  <si>
+    <t>(88,116,153)</t>
+  </si>
+  <si>
+    <t>Taille Font Score</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -241,34 +250,11 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -303,6 +289,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -340,25 +344,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:P13">
-  <autoFilter ref="A1:P13" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{CF5BAF0D-2A1A-45F2-8436-156371C73BFB}" name="Catégorie" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}" name="Tableau1" displayName="Tableau1" ref="A1:Q13">
+  <autoFilter ref="A1:Q13" xr:uid="{047D9689-BF05-4502-AE97-80EADE8AADA6}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{CB34F05D-A392-40F1-B343-180381EBFF50}" name="Afficher" totalsRowLabel="Total" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{CF5BAF0D-2A1A-45F2-8436-156371C73BFB}" name="Catégorie" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{08BE89D9-A157-4F06-A086-DFCD4C59CA11}" name="INFOS"/>
-    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{3B37B40C-DBEB-40E3-9590-405F2A991B75}" name="Texte" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{F99AE48C-BFEA-409C-B0AF-05E54C132F85}" name="Taille Font Score" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{43EE387F-F7F8-44A4-B416-1C991C1828E8}" name="Afficher Texte" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{A3B76A76-22BB-4FCE-BB24-904D08B07977}" name="Couleur Texte" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{4350E952-AA26-4181-A722-64FC122F2526}" name="Couleur Balle"/>
-    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{FBDE0901-02DC-4D23-A925-033B115CD615}" name="Image" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{FC727AA8-9DB1-4BCB-878B-78ACCB013E96}" name="Couleur Rectangle Score"/>
     <tableColumn id="14" xr3:uid="{631E6625-8583-4F25-B9D4-E2EE6798BD97}" name="Couleur Texte Score"/>
-    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon Balle" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{9D1C2EFC-0365-4D39-BEAD-4048F782AF5B}" name="Rayon Balle" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{4F86DC08-4D23-48D4-B800-C3477A97072A}" name="Couleur Interieur Balle"/>
-    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainee" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{25B0C4FB-CC57-4788-8F79-CF3EBC60752A}" name="Taille Contour" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1D6B7618-33F8-4CAA-A676-E20C7BB8498B}" name="Taille Trainee" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D2C41EE0-C6A1-43A0-9560-8145C608F8DB}" name="Taille Font" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{F1E8B700-9EA4-4EE5-BE2B-BF6D2C248379}" name="Acceleration" totalsRowFunction="sum" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,38 +686,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5B4434-761B-4D40-92E9-037B049A5ECC}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" style="4"/>
-    <col min="4" max="4" width="10.6640625" style="3"/>
-    <col min="5" max="5" width="15.46484375" customWidth="1"/>
-    <col min="6" max="6" width="12.265625" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" customWidth="1"/>
-    <col min="8" max="8" width="13.3984375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="23.265625" customWidth="1"/>
-    <col min="10" max="10" width="18.86328125" customWidth="1"/>
-    <col min="11" max="11" width="11.86328125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="6.265625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.86328125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="2"/>
-    <col min="17" max="17" width="10.6640625" style="2"/>
-    <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="20.06640625" customWidth="1"/>
-    <col min="21" max="21" width="12.73046875" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="3"/>
+    <col min="6" max="6" width="15.46484375" customWidth="1"/>
+    <col min="7" max="7" width="12.265625" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.265625" customWidth="1"/>
+    <col min="11" max="11" width="18.86328125" customWidth="1"/>
+    <col min="12" max="12" width="11.86328125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" customWidth="1"/>
+    <col min="14" max="14" width="6.265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.265625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="19.9296875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="2"/>
+    <col min="20" max="20" width="22.33203125" customWidth="1"/>
+    <col min="21" max="21" width="20.06640625" customWidth="1"/>
+    <col min="22" max="22" width="12.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
@@ -721,49 +725,52 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q1"/>
+      <c r="R1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C2" t="s">
@@ -772,46 +779,49 @@
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="b">
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>2</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>10</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>25</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>0.3</v>
       </c>
-      <c r="Q2"/>
+      <c r="R2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C3" t="s">
@@ -820,56 +830,59 @@
       <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="b">
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="2">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>10</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>25</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>0.3</v>
       </c>
-      <c r="Q3"/>
+      <c r="R3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4"/>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C5" t="s">
@@ -878,49 +891,52 @@
       <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
         <v>20</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>2</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>10</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>25</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>0.3</v>
       </c>
-      <c r="Q5"/>
+      <c r="R5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C6" t="s">
@@ -929,49 +945,52 @@
       <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>21</v>
       </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2">
         <v>20</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>10</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>25</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>0.3</v>
       </c>
-      <c r="Q6"/>
+      <c r="R6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C7" t="s">
@@ -980,57 +999,60 @@
       <c r="D7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
         <v>20</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>2</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>10</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>25</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2"/>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C9" t="s">
@@ -1039,48 +1061,51 @@
       <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="2">
         <v>20</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>2</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>10</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>25</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C10" t="s">
@@ -1089,57 +1114,60 @@
       <c r="D10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2">
         <v>20</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>2</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>10</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>25</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2"/>
+      <c r="F11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C12" t="s">
@@ -1148,42 +1176,51 @@
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="2">
+        <v>54</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="2">
         <v>20</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>2</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>10</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>25</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C13" t="s">
@@ -1192,34 +1229,43 @@
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="2">
+        <v>53</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="2">
         <v>20</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>2</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>10</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>25</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout de la possibilité de mettre un commentaire dans le titre
Commentaire pris en priorité par rapport au titre classique
</commit_message>
<xml_diff>
--- a/VideoBalles/ListeBalles.xlsx
+++ b/VideoBalles/ListeBalles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\GitHub\tiktok_manager\VideoBalles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B3666-8773-489A-8641-D35672DEF9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7FD317-354C-4F54-9974-8A9372034EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="2858" windowWidth="16200" windowHeight="9307" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="16200" windowHeight="9308" xr2:uid="{02B7CA46-18BC-42BD-A073-B0E7CB583EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -768,7 +768,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>49</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>49</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>50</v>

</xml_diff>